<commit_message>
benchmark model wide and deep results
</commit_message>
<xml_diff>
--- a/assets/GPT-lite-DeepSpeed/benchmark.xlsx
+++ b/assets/GPT-lite-DeepSpeed/benchmark.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-bmagalhaes\Desktop\brunomaga.github.io\assets\GPT-lite-DeepSpeed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EF7097-D94B-45D8-848C-AE5B1FEFA2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC39667-8994-45F7-AA4D-FB0E788A21F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{5CE2D5A5-40E8-479C-B7CB-2387D3474101}"/>
+    <workbookView xWindow="-16140" yWindow="-21240" windowWidth="16410" windowHeight="14760" firstSheet="1" activeTab="2" xr2:uid="{5CE2D5A5-40E8-479C-B7CB-2387D3474101}"/>
   </bookViews>
   <sheets>
-    <sheet name="benchmark" sheetId="1" r:id="rId1"/>
+    <sheet name="GPTlite" sheetId="1" r:id="rId1"/>
+    <sheet name="Benchmark Wide" sheetId="2" r:id="rId2"/>
+    <sheet name="Benchmark Deep" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Single GPU</t>
   </si>
@@ -47,22 +49,43 @@
     <t>Max Mem Allocated (GB)</t>
   </si>
   <si>
-    <t>DeepSpeed ZeRO3</t>
-  </si>
-  <si>
     <t>DeepSpeedZeRO-Infinity</t>
   </si>
   <si>
     <t>DeepSpeed ZerRO1 Pipeline</t>
   </si>
   <si>
-    <t>Input Size per GPU</t>
-  </si>
-  <si>
     <t>Distributed Data Parallel</t>
   </si>
   <si>
     <t>Throughput (samples/sec)</t>
+  </si>
+  <si>
+    <t>DeepSpeed ZeRO-3</t>
+  </si>
+  <si>
+    <t>DeepSpeed ZeRO-1</t>
+  </si>
+  <si>
+    <t>DeepSpeed ZeRO-2</t>
+  </si>
+  <si>
+    <t>Avg Mem Allocated (GB)</t>
+  </si>
+  <si>
+    <t>DeepSpeed ZeRO-1 Pipeline</t>
+  </si>
+  <si>
+    <t>DeepSpeed ZeRO-Infinity</t>
+  </si>
+  <si>
+    <t>W=8192, L=3</t>
+  </si>
+  <si>
+    <t>W=256, L=1024</t>
+  </si>
+  <si>
+    <t>Throughput (10K samples/sec)</t>
   </si>
 </sst>
 </file>
@@ -152,7 +175,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>benchmark!$A$6</c:f>
+              <c:f>GPTlite!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -230,9 +253,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>benchmark!$B$1:$E$1</c:f>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
@@ -241,19 +264,16 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Input Size per GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>benchmark!$B$6:$E$6</c:f>
+              <c:f>GPTlite!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -268,7 +288,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>benchmark!$A$5</c:f>
+              <c:f>GPTlite!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -346,9 +366,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>benchmark!$B$1:$E$1</c:f>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
@@ -357,19 +377,16 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Input Size per GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>benchmark!$B$5:$E$5</c:f>
+              <c:f>GPTlite!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -384,11 +401,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>benchmark!$A$4</c:f>
+              <c:f>GPTlite!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO3</c:v>
+                  <c:v>DeepSpeed ZeRO-3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -462,9 +479,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>benchmark!$B$1:$E$1</c:f>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
@@ -473,19 +490,16 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Input Size per GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>benchmark!$B$4:$E$4</c:f>
+              <c:f>GPTlite!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>10.71</c:v>
                 </c:pt>
@@ -494,9 +508,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -512,7 +523,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>benchmark!$A$3</c:f>
+              <c:f>GPTlite!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -590,9 +601,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>benchmark!$B$1:$E$1</c:f>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
@@ -601,19 +612,16 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Input Size per GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>benchmark!$B$3:$E$3</c:f>
+              <c:f>GPTlite!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>12.57</c:v>
                 </c:pt>
@@ -622,9 +630,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.4499999999999993</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -640,7 +645,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>benchmark!$A$2</c:f>
+              <c:f>GPTlite!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -718,9 +723,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>benchmark!$B$1:$E$1</c:f>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
@@ -729,19 +734,16 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Input Size per GPU</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>benchmark!$B$2:$E$2</c:f>
+              <c:f>GPTlite!$B$2:$D$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.63</c:v>
                 </c:pt>
@@ -750,9 +752,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.4499999999999993</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -963,7 +962,1864 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Wide benchmark model (W=8192, L=3)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1 Pipeline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6783-47FD-8B50-B30016C9542F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-Infinity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.1639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6783-47FD-8B50-B30016C9542F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.6319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6783-47FD-8B50-B30016C9542F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.76100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6783-47FD-8B50-B30016C9542F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.71099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6783-47FD-8B50-B30016C9542F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distributed Data Parallel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.5489999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-6783-47FD-8B50-B30016C9542F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="388047104"/>
+        <c:axId val="345613824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="388047104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345613824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="345613824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388047104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.7117083394528379E-2"/>
+          <c:y val="0.93405171288902489"/>
+          <c:w val="0.67591730808929784"/>
+          <c:h val="6.5948484848484853E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Deep benchmark</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> model (W=256, L=1024)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1 Pipeline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-7CEA-4C2F-B755-15A8E344247C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-Infinity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.20399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-7CEA-4C2F-B755-15A8E344247C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-7CEA-4C2F-B755-15A8E344247C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7CEA-4C2F-B755-15A8E344247C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.60099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7CEA-4C2F-B755-15A8E344247C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distributed Data Parallel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.7270000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7CEA-4C2F-B755-15A8E344247C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="388047104"/>
+        <c:axId val="345613824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="388047104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345613824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="345613824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388047104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.7117083394528379E-2"/>
+          <c:y val="0.93405171288902489"/>
+          <c:w val="0.67591730808929784"/>
+          <c:h val="6.5948484848484853E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1508,6 +3364,1016 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1518,10 +4384,10 @@
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>647701</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1670050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1533,6 +4399,92 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1657350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>111900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23ED2034-8ECF-4FEA-939F-F9F7EBD14FBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1682750</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>35700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4881FF-AFAB-450D-8D23-168D761F6E8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1866,10 +4818,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBAB1DA-DD82-4512-8D36-0FA776F72118}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1.63</v>
+      </c>
+      <c r="C2">
+        <v>2.27</v>
+      </c>
+      <c r="D2">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>12.57</v>
+      </c>
+      <c r="C3">
+        <v>2.27</v>
+      </c>
+      <c r="D3">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>10.71</v>
+      </c>
+      <c r="C4">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="D4">
+        <v>9.6</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8454C2-D505-4BE9-A00C-2F5F82517839}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1878,92 +4928,230 @@
     <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1"/>
+      <c r="E1" s="1"/>
       <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>1.63</v>
+        <v>1.5489999999999999</v>
       </c>
       <c r="C2">
-        <v>2.27</v>
+        <v>2.39</v>
       </c>
       <c r="D2">
-        <v>9.4499999999999993</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
+        <v>3.77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="C3">
+        <v>1.17</v>
+      </c>
+      <c r="D3">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="C4">
+        <v>1.17</v>
+      </c>
+      <c r="D4">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>12.57</v>
-      </c>
-      <c r="C3">
-        <v>2.27</v>
-      </c>
-      <c r="D3">
-        <v>9.4499999999999993</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="B5">
+        <f>1.632</f>
+        <v>1.6319999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.61</v>
+      </c>
+      <c r="D5">
+        <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>10.71</v>
-      </c>
-      <c r="C4">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D4">
-        <v>9.6</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D6">
+        <v>1.41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8A79F4-1607-4AB9-B9C5-1A44146CDC76}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1.7270000000000001</v>
+      </c>
+      <c r="C2">
+        <v>1.53</v>
+      </c>
+      <c r="D2">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="C3">
+        <v>0.71</v>
+      </c>
+      <c r="D3">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="C4">
+        <v>0.71</v>
+      </c>
+      <c r="D4">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.253</v>
+      </c>
+      <c r="C5">
+        <v>0.84</v>
+      </c>
+      <c r="D5">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.52</v>
+      </c>
+      <c r="D6">
+        <v>4.53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added benchmark without pipelining
</commit_message>
<xml_diff>
--- a/assets/GPT-lite-DeepSpeed/benchmark.xlsx
+++ b/assets/GPT-lite-DeepSpeed/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-bmagalhaes\Desktop\brunomaga.github.io\assets\GPT-lite-DeepSpeed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA40F03-6FE9-4B08-81D2-186749CE3F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8CA72F-027E-4EBC-86D7-7CF01185D427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16140" yWindow="-21240" windowWidth="16410" windowHeight="14760" tabRatio="669" activeTab="2" xr2:uid="{5CE2D5A5-40E8-479C-B7CB-2387D3474101}"/>
+    <workbookView xWindow="-16320" yWindow="-22185" windowWidth="16440" windowHeight="29040" tabRatio="669" activeTab="1" xr2:uid="{5CE2D5A5-40E8-479C-B7CB-2387D3474101}"/>
   </bookViews>
   <sheets>
     <sheet name="GPTlite" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t>Max Mem Allocated (GB)</t>
   </si>
@@ -73,7 +73,10 @@
     <t>Throughput (10K samples/sec)</t>
   </si>
   <si>
-    <t>GPT-lite</t>
+    <t>GPT-lite small</t>
+  </si>
+  <si>
+    <t>Throughput (samples/sec)</t>
   </si>
 </sst>
 </file>
@@ -172,11 +175,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>GPT</a:t>
+              <a:t>GPT-lite</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> lite model (small)</a:t>
+              <a:t> model (small)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -223,7 +226,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GPTlite!$A$7</c:f>
+              <c:f>GPTlite!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -305,7 +308,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
+                  <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Avg Mem Allocated (GB)</c:v>
@@ -318,7 +321,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GPTlite!$B$7:$D$7</c:f>
+              <c:f>GPTlite!$B$2:$D$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -327,7 +330,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-F32D-435F-BF91-9D7DA7FFEBED}"/>
+              <c16:uniqueId val="{00000000-D7BC-4C73-9384-8E03114129B3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -336,7 +339,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GPTlite!$A$6</c:f>
+              <c:f>GPTlite!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -418,7 +421,7 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
+                  <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Avg Mem Allocated (GB)</c:v>
@@ -431,25 +434,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GPTlite!$B$6:$D$6</c:f>
+              <c:f>GPTlite!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.20399999999999999</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52</c:v>
+                  <c:v>2.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.53</c:v>
+                  <c:v>9.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-F32D-435F-BF91-9D7DA7FFEBED}"/>
+              <c16:uniqueId val="{00000001-D7BC-4C73-9384-8E03114129B3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -458,7 +461,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>GPTlite!$A$5</c:f>
+              <c:f>GPTlite!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -540,7 +543,129 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
+                  <c:v>Throughput (samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GPTlite!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3699999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D7BC-4C73-9384-8E03114129B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GPTlite!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (samples/sec)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Avg Mem Allocated (GB)</c:v>
@@ -558,40 +683,673 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.253</c:v>
+                  <c:v>10.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84</c:v>
+                  <c:v>2.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.84</c:v>
+                  <c:v>9.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-F32D-435F-BF91-9D7DA7FFEBED}"/>
+              <c16:uniqueId val="{0000000C-D7BC-4C73-9384-8E03114129B3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:idx val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>GPTlite!$A$4</c:f>
+              <c:f>GPTlite!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-2</c:v>
+                  <c:v>DeepSpeed ZeRO-1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GPTlite!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-D7BC-4C73-9384-8E03114129B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GPTlite!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distributed Data Parallel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>GPTlite!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GPTlite!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-D7BC-4C73-9384-8E03114129B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="388047104"/>
+        <c:axId val="345613824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="388047104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345613824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="345613824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388047104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.7117083394528379E-2"/>
+          <c:y val="0.93405171288902489"/>
+          <c:w val="0.67559472030485901"/>
+          <c:h val="6.5948368596363716E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Wide benchmark model (W=8192, L=3)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1 Pipeline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E405-45C5-B847-3310226F5C48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-Infinity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -658,7 +1416,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>GPTlite!$B$1:$D$1</c:f>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -675,45 +1433,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GPTlite!$B$4:$D$4</c:f>
+              <c:f>'Benchmark Wide'!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.498</c:v>
+                  <c:v>1.1639999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.72</c:v>
+                  <c:v>1.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F32D-435F-BF91-9D7DA7FFEBED}"/>
+              <c16:uniqueId val="{00000001-E405-45C5-B847-3310226F5C48}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="4"/>
+          <c:idx val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>GPTlite!$A$3</c:f>
+              <c:f>'Benchmark Wide'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-1</c:v>
+                  <c:v>DeepSpeed ZeRO-3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -780,7 +1538,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>GPTlite!$B$1:$D$1</c:f>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -797,25 +1555,269 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GPTlite!$B$3:$D$3</c:f>
+              <c:f>'Benchmark Wide'!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.60099999999999998</c:v>
+                  <c:v>1.853</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.72</c:v>
+                  <c:v>1.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F32D-435F-BF91-9D7DA7FFEBED}"/>
+              <c16:uniqueId val="{00000000-E405-45C5-B847-3310226F5C48}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.72799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FDB3-4845-A32C-B9D68D2FEBCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.79400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FDB3-4845-A32C-B9D68D2FEBCC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -824,7 +1826,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>GPTlite!$A$2</c:f>
+              <c:f>'Benchmark Wide'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -836,6 +1838,517 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Wide'!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FDB3-4845-A32C-B9D68D2FEBCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="388047104"/>
+        <c:axId val="345613824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="388047104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="345613824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="345613824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388047104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.7117083394528379E-2"/>
+          <c:y val="0.93405171288902489"/>
+          <c:w val="0.67610260541094158"/>
+          <c:h val="6.5948219079617995E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Wide benchmark model (W=8192, L=3)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1 Pipeline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2735-473C-8B81-084F2428B76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-Infinity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -902,7 +2415,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>GPTlite!$B$1:$D$1</c:f>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -919,7 +2432,495 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GPTlite!$B$2:$D$2</c:f>
+              <c:f>'Benchmark Deep'!$B$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.20399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2735-473C-8B81-084F2428B76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2735-473C-8B81-084F2428B76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-2735-473C-8B81-084F2428B76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DeepSpeed ZeRO-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.60099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-2735-473C-8B81-084F2428B76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distributed Data Parallel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Throughput (10K samples/sec)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avg Mem Allocated (GB)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Max Mem Allocated (GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Benchmark Deep'!$B$7:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -937,7 +2938,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F32D-435F-BF91-9D7DA7FFEBED}"/>
+              <c16:uniqueId val="{0000000B-2735-473C-8B81-084F2428B76E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1141,1838 +3142,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Wide benchmark model (W=8192, L=3)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-1 Pipeline</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Wide'!$B$7:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E405-45C5-B847-3310226F5C48}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-Infinity</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Wide'!$B$6:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.1639999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.41</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E405-45C5-B847-3310226F5C48}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Wide'!$B$5:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.6319999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.61</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0699999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E405-45C5-B847-3310226F5C48}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Wide'!$B$4:$D$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.76100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.88</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6783-47FD-8B50-B30016C9542F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Wide'!$B$3:$D$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.71099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0099999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6783-47FD-8B50-B30016C9542F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Distributed Data Parallel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Wide'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Wide'!$B$2:$D$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.5489999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.39</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.77</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6783-47FD-8B50-B30016C9542F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="388047104"/>
-        <c:axId val="345613824"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="388047104"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="345613824"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="345613824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="388047104"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.7117083394528379E-2"/>
-          <c:y val="0.93405171288902489"/>
-          <c:w val="0.67591730808929784"/>
-          <c:h val="6.594838734095769E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Deep benchmark</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> model (W=256, L=1024)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-1 Pipeline</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Deep'!$B$7:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-49D9-4C3E-A989-CAC4E0B4C28F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-Infinity</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Deep'!$B$6:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.20399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.53</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-49D9-4C3E-A989-CAC4E0B4C28F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Deep'!$B$5:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.253</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.84</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-49D9-4C3E-A989-CAC4E0B4C28F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Deep'!$B$4:$D$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.498</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.72</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-7CEA-4C2F-B755-15A8E344247C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DeepSpeed ZeRO-1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Deep'!$B$3:$D$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.60099999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.72</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-7CEA-4C2F-B755-15A8E344247C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Distributed Data Parallel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Benchmark Deep'!$B$1:$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Throughput (10K samples/sec)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Avg Mem Allocated (GB)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Max Mem Allocated (GB)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Benchmark Deep'!$B$2:$D$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.7270000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.53</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.53</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-7CEA-4C2F-B755-15A8E344247C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="388047104"/>
-        <c:axId val="345613824"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="388047104"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="345613824"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="345613824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="388047104"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.7117083394528379E-2"/>
-          <c:y val="0.93405171288902489"/>
-          <c:w val="0.67591730808929784"/>
-          <c:h val="6.5948484848484853E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4613,22 +4782,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:colOff>1244600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>105550</xdr:rowOff>
+      <xdr:rowOff>775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46A3F170-02DF-4349-85FB-48574102534E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2283713-4C87-4A40-8038-F76F4E458A0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4656,15 +4825,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>27209</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>13904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1543050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>159525</xdr:rowOff>
+      <xdr:colOff>1475009</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>176604</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4699,22 +4868,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1682750</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>35700</xdr:rowOff>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>159525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4881FF-AFAB-450D-8D23-168D761F6E8E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B4DF4F3-D4F2-41D8-B773-D7776A381426}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5056,14 +5225,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBAB1DA-DD82-4512-8D36-0FA776F72118}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="122" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.1796875" customWidth="1"/>
@@ -5078,7 +5247,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -5093,77 +5262,77 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1.7270000000000001</v>
-      </c>
-      <c r="C2">
-        <v>1.53</v>
-      </c>
-      <c r="D2">
-        <v>5.53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.60099999999999998</v>
+        <v>6.2</v>
       </c>
       <c r="C3">
-        <v>0.71</v>
+        <v>2.35</v>
       </c>
       <c r="D3">
-        <v>4.72</v>
+        <v>9.16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.498</v>
+        <v>7.1</v>
       </c>
       <c r="C4">
-        <v>0.71</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="D4">
-        <v>4.72</v>
+        <v>9.3699999999999992</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0.253</v>
+        <v>10.44</v>
       </c>
       <c r="C5">
-        <v>0.84</v>
+        <v>2.71</v>
       </c>
       <c r="D5">
-        <v>4.84</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>0.20399999999999999</v>
+        <v>11.07</v>
       </c>
       <c r="C6">
-        <v>0.52</v>
+        <v>2.71</v>
       </c>
       <c r="D6">
-        <v>4.53</v>
+        <v>9.61</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>11.45</v>
+      </c>
+      <c r="C7">
+        <v>3.24</v>
+      </c>
+      <c r="D7">
+        <v>10.16</v>
       </c>
     </row>
   </sheetData>
@@ -5177,8 +5346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8454C2-D505-4BE9-A00C-2F5F82517839}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5214,41 +5383,33 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1.5489999999999999</v>
-      </c>
-      <c r="C2">
-        <v>2.39</v>
-      </c>
-      <c r="D2">
-        <v>3.77</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.71099999999999997</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="C3">
-        <v>1.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D3">
-        <v>2.0099999999999998</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.76100000000000001</v>
+        <f>1.853</f>
+        <v>1.853</v>
       </c>
       <c r="C4">
-        <v>1.17</v>
+        <v>0.61</v>
       </c>
       <c r="D4">
         <v>1.88</v>
@@ -5256,36 +5417,44 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <f>1.632</f>
-        <v>1.6319999999999999</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="C5">
-        <v>0.61</v>
+        <v>1.17</v>
       </c>
       <c r="D5">
-        <v>2.0699999999999998</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>1.1639999999999999</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="C6">
-        <v>0.14000000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="D6">
-        <v>1.41</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1.57</v>
+      </c>
+      <c r="C7">
+        <v>2.39</v>
+      </c>
+      <c r="D7">
+        <v>3.89</v>
       </c>
     </row>
   </sheetData>
@@ -5298,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8A79F4-1607-4AB9-B9C5-1A44146CDC76}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5335,77 +5504,77 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1.7270000000000001</v>
-      </c>
-      <c r="C2">
-        <v>1.53</v>
-      </c>
-      <c r="D2">
-        <v>5.53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>0.60099999999999998</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="C3">
-        <v>0.71</v>
+        <v>0.52</v>
       </c>
       <c r="D3">
-        <v>4.72</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.498</v>
+        <v>0.253</v>
       </c>
       <c r="C4">
-        <v>0.71</v>
+        <v>0.84</v>
       </c>
       <c r="D4">
-        <v>4.72</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0.253</v>
+        <v>0.498</v>
       </c>
       <c r="C5">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
       <c r="D5">
-        <v>4.84</v>
+        <v>4.72</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>0.20399999999999999</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="C6">
-        <v>0.52</v>
+        <v>0.71</v>
       </c>
       <c r="D6">
-        <v>4.53</v>
+        <v>4.72</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1.7270000000000001</v>
+      </c>
+      <c r="C7">
+        <v>1.53</v>
+      </c>
+      <c r="D7">
+        <v>5.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new benchmark deep img
</commit_message>
<xml_diff>
--- a/assets/GPT-lite-DeepSpeed/benchmark.xlsx
+++ b/assets/GPT-lite-DeepSpeed/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-bmagalhaes\Desktop\brunomaga.github.io\assets\GPT-lite-DeepSpeed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8CA72F-027E-4EBC-86D7-7CF01185D427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C958C7-E8F8-4DDB-9A3E-475776E60A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-22185" windowWidth="16440" windowHeight="29040" tabRatio="669" activeTab="1" xr2:uid="{5CE2D5A5-40E8-479C-B7CB-2387D3474101}"/>
+    <workbookView xWindow="-16320" yWindow="-22185" windowWidth="16440" windowHeight="29040" tabRatio="669" activeTab="2" xr2:uid="{5CE2D5A5-40E8-479C-B7CB-2387D3474101}"/>
   </bookViews>
   <sheets>
     <sheet name="GPTlite" sheetId="1" r:id="rId1"/>
@@ -2178,7 +2178,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Wide benchmark model (W=8192, L=3)</a:t>
+              <a:t>Deep benchmark model (W=8192, L=3)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3077,8 +3077,8 @@
           <c:yMode val="edge"/>
           <c:x val="4.7117083394528379E-2"/>
           <c:y val="0.93405171288902489"/>
-          <c:w val="0.67591730808929784"/>
-          <c:h val="6.594838734095769E-2"/>
+          <c:w val="0.67645726631105274"/>
+          <c:h val="6.5948520107968242E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4868,15 +4868,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>24634</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>172434</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:colOff>1472434</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>159525</xdr:rowOff>
+      <xdr:rowOff>157663</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5346,7 +5346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8454C2-D505-4BE9-A00C-2F5F82517839}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
+    <sheetView zoomScale="123" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -5467,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8A79F4-1607-4AB9-B9C5-1A44146CDC76}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="122" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>